<commit_message>
Finsh: unit test, mock model test, README added, UML & Testing update, example run，100%style Done!
</commit_message>
<xml_diff>
--- a/Milestone2_TestingPlan.xlsx
+++ b/Milestone2_TestingPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zackxue/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zackxue/Desktop/CS5010PDP_23Fall/MilestoneProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C75342C-FA3E-7B4C-848F-62CF794C3754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1303627E-EEF7-054D-9E1B-87C3C7AD1ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21040" windowWidth="30420" windowHeight="20660" activeTab="1" xr2:uid="{A1608EE0-BA0E-7941-8500-47259AB4F5B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="384">
   <si>
     <t>DrLucky</t>
   </si>
@@ -578,10 +578,6 @@
     <t>BufferedImage</t>
   </si>
   <si>
-    <t>Milestone2_Controller
-Class Name</t>
-  </si>
-  <si>
     <t>testControllerConsoleStartGameSuccess</t>
   </si>
   <si>
@@ -1003,6 +999,203 @@
   </si>
   <si>
     <t>Controller: WorldController_Console_Implement</t>
+  </si>
+  <si>
+    <t>Model: Mock_World Ms2MockWorldTest</t>
+  </si>
+  <si>
+    <t>testGetNeighborsRoomList</t>
+  </si>
+  <si>
+    <t>testGetWorldName</t>
+  </si>
+  <si>
+    <t>testGetTotalOfRoom</t>
+  </si>
+  <si>
+    <t>testGetTotalOfItem</t>
+  </si>
+  <si>
+    <t>testGetOneRoomInfo</t>
+  </si>
+  <si>
+    <t>testMoveDrLucky</t>
+  </si>
+  <si>
+    <t>testCreateGraphBufferedImage</t>
+  </si>
+  <si>
+    <t>testPrintWorldNeighborMap</t>
+  </si>
+  <si>
+    <t>testGetDrLuckyInfo</t>
+  </si>
+  <si>
+    <t>testPrintAllRoomInfo</t>
+  </si>
+  <si>
+    <t>testAddOnePlayer</t>
+  </si>
+  <si>
+    <t>testSetTotalAllowedTurns</t>
+  </si>
+  <si>
+    <t>testSetTotalAllowedPlayers</t>
+  </si>
+  <si>
+    <t>testCmdComputerPlayerAction</t>
+  </si>
+  <si>
+    <t>testCmdPlayerMove</t>
+  </si>
+  <si>
+    <t>testCmdPlayerLook</t>
+  </si>
+  <si>
+    <t>testCmdPlayerPick</t>
+  </si>
+  <si>
+    <t>testCheckGameOver</t>
+  </si>
+  <si>
+    <t>testGetAllPlayerNames</t>
+  </si>
+  <si>
+    <t>testGetAllPlayerInfo</t>
+  </si>
+  <si>
+    <t>testGetAllRoomNames</t>
+  </si>
+  <si>
+    <t>testGetOnePlayerAndRoomInfo</t>
+  </si>
+  <si>
+    <t>testGetOnePlayerCurrentRoomName</t>
+  </si>
+  <si>
+    <t>testGetCurrentPlayerName</t>
+  </si>
+  <si>
+    <t>testIsCurrentPlayerComputer</t>
+  </si>
+  <si>
+    <t>testGetCurrentPlayerIndex</t>
+  </si>
+  <si>
+    <t>testGetCurrentTurnNumber</t>
+  </si>
+  <si>
+    <t>Check gameLog make sure the correct function is called and executed!</t>
+  </si>
+  <si>
+    <t>Playe look string</t>
+  </si>
+  <si>
+    <t>Player move String</t>
+  </si>
+  <si>
+    <t>Playe pick string</t>
+  </si>
+  <si>
+    <t>getNeighborsRoomList("Room1")</t>
+  </si>
+  <si>
+    <t>getWorldName()</t>
+  </si>
+  <si>
+    <t>getTotalOfRoom()</t>
+  </si>
+  <si>
+    <t>getTotalOfItem()</t>
+  </si>
+  <si>
+    <t>getOneRoomInfo("Room1")</t>
+  </si>
+  <si>
+    <t>createGraphBufferedImage();</t>
+  </si>
+  <si>
+    <t>printWorldNeighborMap();</t>
+  </si>
+  <si>
+    <t>getDrLuckyInfo();</t>
+  </si>
+  <si>
+    <t>printAllRoomInfo();</t>
+  </si>
+  <si>
+    <t>addOnePlayer("Player1", 0, false, 5);</t>
+  </si>
+  <si>
+    <t>Player name, limit, room, computer or not?</t>
+  </si>
+  <si>
+    <t>setTotalAllowedTurns(10);</t>
+  </si>
+  <si>
+    <t>setTotalAllowedPlayers(4);</t>
+  </si>
+  <si>
+    <t>cmdComputerPlayerAction();</t>
+  </si>
+  <si>
+    <t>cmdPlayerMove("Room2");</t>
+  </si>
+  <si>
+    <t>cmdPlayerLook();</t>
+  </si>
+  <si>
+    <t>cmdPlayerPick("Item1");</t>
+  </si>
+  <si>
+    <t>world.setTotalAllowedTurns(5);
+    world.cmdComputerPlayerAction();
+    world.cmdComputerPlayerAction();
+    world.cmdComputerPlayerAction();
+    world.cmdComputerPlayerAction();</t>
+  </si>
+  <si>
+    <t>combined different command input to run game until end.</t>
+  </si>
+  <si>
+    <t>getAllPlayerNames();</t>
+  </si>
+  <si>
+    <t>getAllPlayerInfo();</t>
+  </si>
+  <si>
+    <t>getAllRoomNames();</t>
+  </si>
+  <si>
+    <t>getOnePlayerAndRoomInfo("Player1");</t>
+  </si>
+  <si>
+    <t>getOnePlayerCurrentRoomName("Player1");</t>
+  </si>
+  <si>
+    <t>getCurrentPlayerName();</t>
+  </si>
+  <si>
+    <t>isCurrentPlayerComputer();</t>
+  </si>
+  <si>
+    <t>True or false depending currently player type</t>
+  </si>
+  <si>
+    <t>getCurrentPlayerIndex();</t>
+  </si>
+  <si>
+    <t>getCurrentTurnNumber();</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Class Name：</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone2_Controller (Author: Zack Xue)
+</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1144,23 +1337,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2668,13 +2852,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14BACED-A339-4394-BEA2-4546E874292B}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2691,7 +2875,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>179</v>
+        <v>383</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>173</v>
@@ -2714,622 +2898,624 @@
     </row>
     <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="B2" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>316</v>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="16" t="s">
-        <v>188</v>
+      <c r="B4" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="16" t="s">
-        <v>190</v>
+      <c r="F4" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="16" t="s">
-        <v>191</v>
+      <c r="B5" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="17" t="s">
-        <v>192</v>
+      <c r="F5" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="17" t="s">
-        <v>193</v>
+      <c r="B6" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="17" t="s">
-        <v>207</v>
+      <c r="B7" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="17" t="s">
-        <v>197</v>
+      <c r="B8" s="11" t="s">
+        <v>196</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="17" t="s">
-        <v>210</v>
+      <c r="B9" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>218</v>
+        <v>260</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="17" t="s">
-        <v>212</v>
+      <c r="B10" s="11" t="s">
+        <v>211</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>219</v>
+        <v>248</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="17" t="s">
-        <v>213</v>
+      <c r="B11" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="17" t="s">
-        <v>220</v>
+      <c r="F11" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="17" t="s">
-        <v>214</v>
+      <c r="B12" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="17" t="s">
-        <v>215</v>
+      <c r="B13" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="17" t="s">
-        <v>229</v>
+      <c r="F13" s="11" t="s">
+        <v>228</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="17" t="s">
-        <v>221</v>
+      <c r="B14" s="11" t="s">
+        <v>220</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>225</v>
+        <v>248</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>224</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="17" t="s">
-        <v>222</v>
+      <c r="B15" s="11" t="s">
+        <v>221</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="17" t="s">
-        <v>226</v>
+      <c r="F15" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="17" t="s">
-        <v>223</v>
+      <c r="B16" s="11" t="s">
+        <v>222</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="17" t="s">
-        <v>227</v>
+      <c r="F16" s="11" t="s">
+        <v>226</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="17" t="s">
-        <v>224</v>
+      <c r="B17" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="17" t="s">
-        <v>228</v>
+      <c r="F17" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="B18" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19" t="s">
+      <c r="G18" s="17" t="s">
         <v>239</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="17" t="s">
-        <v>236</v>
+      <c r="B19" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="17" t="s">
-        <v>235</v>
+      <c r="F19" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="D20" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="18" t="s">
+      <c r="G20" s="13" t="s">
         <v>233</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="17" t="s">
-        <v>243</v>
+      <c r="B21" s="11" t="s">
+        <v>242</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F21" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="G22" s="13" t="s">
         <v>246</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="17" t="s">
-        <v>248</v>
+      <c r="B23" s="11" t="s">
+        <v>247</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>254</v>
+        <v>249</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>253</v>
       </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>256</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="17" t="s">
-        <v>265</v>
+      <c r="B25" s="11" t="s">
+        <v>264</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>218</v>
+        <v>258</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="18" t="s">
-        <v>266</v>
+      <c r="B26" s="10" t="s">
+        <v>265</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E26" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>259</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="18" t="s">
-        <v>267</v>
+      <c r="B27" s="10" t="s">
+        <v>266</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E27" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="17" t="s">
-        <v>268</v>
+      <c r="B28" s="11" t="s">
+        <v>267</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="11" t="s">
         <v>269</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="17" t="s">
-        <v>270</v>
       </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="18" t="s">
-        <v>271</v>
+      <c r="B29" s="10" t="s">
+        <v>270</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="18" t="s">
-        <v>246</v>
+      <c r="F29" s="10" t="s">
+        <v>245</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="17" t="s">
-        <v>273</v>
+      <c r="B30" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="17" t="s">
+      <c r="G30" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="17" t="s">
-        <v>277</v>
+      <c r="B31" s="11" t="s">
+        <v>276</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="17" t="s">
-        <v>201</v>
+      <c r="F31" s="11" t="s">
+        <v>200</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="F32" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="F32" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="G32" s="20"/>
+      <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
-      <c r="B33" s="17" t="s">
-        <v>285</v>
+      <c r="B33" s="11" t="s">
+        <v>284</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G34" s="13"/>
     </row>
     <row r="35" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="10" t="s">
         <v>286</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="17" t="s">
-        <v>288</v>
+      <c r="B36" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="17" t="s">
-        <v>290</v>
       </c>
       <c r="G36" s="2" t="b">
         <v>0</v>
@@ -3337,16 +3523,16 @@
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="17" t="s">
-        <v>291</v>
+      <c r="B37" s="11" t="s">
+        <v>290</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="17" t="s">
-        <v>292</v>
+      <c r="F37" s="11" t="s">
+        <v>291</v>
       </c>
       <c r="G37" s="2" t="b">
         <v>1</v>
@@ -3354,133 +3540,466 @@
     </row>
     <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="17" t="s">
-        <v>293</v>
+      <c r="B38" s="11" t="s">
+        <v>292</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="17" t="s">
+      <c r="G38" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="17" t="s">
-        <v>297</v>
+      <c r="B39" s="11" t="s">
+        <v>296</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="17" t="s">
-        <v>300</v>
+      <c r="B40" s="11" t="s">
+        <v>299</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>303</v>
       </c>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="17" t="s">
-        <v>308</v>
+      <c r="B42" s="11" t="s">
+        <v>307</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="17" t="s">
-        <v>309</v>
+      <c r="F42" s="11" t="s">
+        <v>308</v>
       </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="18" t="s">
-        <v>310</v>
+      <c r="B43" s="10" t="s">
+        <v>309</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="18" t="s">
+      <c r="F43" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="18" t="s">
-        <v>312</v>
+      <c r="B44" s="10" t="s">
+        <v>311</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B59" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B60" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B70" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>